<commit_message>
agr sim acho que está tudo da página de admin sem o uso de WebSockets next step: tratar dos WebSockets e das votações
</commit_message>
<xml_diff>
--- a/sd_checklist_meta2.xlsx
+++ b/sd_checklist_meta2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raul/Home/Git/SDIST/projeto_meta_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao_\Documents\João Filipe\Universidade\4º Ano\2º Semestre\SD\Projeto-SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB9790F-7E8D-044B-BC5E-A02A9F605344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0498587A-0301-46B4-8C62-01BCC130E531}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="460" windowWidth="27820" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-21" sheetId="3" r:id="rId1"/>
@@ -184,7 +184,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -209,7 +209,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,6 +219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,7 +285,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -302,22 +308,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="15">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -707,7 +719,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -751,7 +763,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -775,25 +787,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BR47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="121" zoomScaleNormal="121" zoomScalePageLayoutView="121" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" zoomScalePageLayoutView="121" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="75.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" s="1" customFormat="1" ht="18">
       <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:70" s="5" customFormat="1">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -801,7 +813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:70" s="5" customFormat="1">
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
@@ -809,7 +821,7 @@
         <v>2017987654</v>
       </c>
     </row>
-    <row r="5" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:70" s="5" customFormat="1">
       <c r="A5" s="5">
         <f>A6+A21+A25+A31</f>
         <v>100</v>
@@ -1074,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="BO5" s="5">
-        <f t="shared" ref="BO5:CT5" si="2">BO6+BO21+BO25+BO31+BO36+BO41</f>
+        <f t="shared" ref="BO5:BR5" si="2">BO6+BO21+BO25+BO31+BO36+BO41</f>
         <v>0</v>
       </c>
       <c r="BP5" s="5">
@@ -1090,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:70" s="1" customFormat="1" ht="18">
       <c r="A6" s="1">
         <f>SUM(A7:A20)</f>
         <v>57</v>
@@ -1371,84 +1383,84 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A9" s="3">
         <v>5</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A10" s="3">
         <v>5</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A11" s="3">
         <v>5</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A12" s="3">
         <v>5</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A13" s="3">
         <v>5</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A14" s="3">
         <v>7</v>
       </c>
@@ -1459,18 +1471,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A15" s="3">
         <v>5</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A16" s="3">
         <v>5</v>
       </c>
@@ -1481,18 +1493,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A17" s="3">
         <v>5</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A18" s="3">
         <v>0</v>
       </c>
@@ -1503,7 +1515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A19" s="3">
         <v>0</v>
       </c>
@@ -1514,7 +1526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A20" s="3">
         <v>0</v>
       </c>
@@ -1525,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:70" s="1" customFormat="1" ht="18">
       <c r="A21" s="1">
         <f>SUM(A22:A24)</f>
         <v>15</v>
@@ -1806,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A22" s="3">
         <v>5</v>
       </c>
@@ -1817,7 +1829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A23" s="3">
         <v>5</v>
       </c>
@@ -1828,7 +1840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A24" s="3">
         <v>5</v>
       </c>
@@ -1839,7 +1851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:70" s="1" customFormat="1" ht="18">
       <c r="A25" s="1">
         <f>SUM(A26:A30)</f>
         <v>20</v>
@@ -2120,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A26" s="3">
         <v>5</v>
       </c>
@@ -2131,7 +2143,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A27" s="3">
         <v>5</v>
       </c>
@@ -2142,7 +2154,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A28" s="3">
         <v>5</v>
       </c>
@@ -2153,7 +2165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A29" s="3">
         <v>5</v>
       </c>
@@ -2164,7 +2176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A30" s="3">
         <v>0</v>
       </c>
@@ -2175,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:70" s="1" customFormat="1" ht="18">
       <c r="A31" s="1">
         <f>SUM(A32:A35)</f>
         <v>8</v>
@@ -2440,7 +2452,7 @@
         <v>0</v>
       </c>
       <c r="BO31" s="1">
-        <f t="shared" ref="BO31:CT31" si="11">SUM(BO32:BO35)</f>
+        <f t="shared" ref="BO31:BR31" si="11">SUM(BO32:BO35)</f>
         <v>0</v>
       </c>
       <c r="BP31" s="1">
@@ -2456,7 +2468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A32" s="3">
         <v>2</v>
       </c>
@@ -2467,7 +2479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A33" s="3">
         <v>2</v>
       </c>
@@ -2478,7 +2490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A34" s="3">
         <v>2</v>
       </c>
@@ -2489,7 +2501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A35" s="3">
         <v>2</v>
       </c>
@@ -2500,7 +2512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:70" s="1" customFormat="1" ht="18">
       <c r="B36" s="2" t="s">
         <v>10</v>
       </c>
@@ -2777,27 +2789,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="B37" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="B38" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="B39" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="B40" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:70" s="1" customFormat="1" ht="18">
       <c r="B41" s="2" t="s">
         <v>12</v>
       </c>
@@ -3074,32 +3086,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="B42" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="B43" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="B44" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="B45" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="B46" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:70" s="1" customFormat="1" ht="18">
       <c r="B47" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
adicionei um interceptor para os users normais não acederem a páginas de admin next step: começar com websockets
</commit_message>
<xml_diff>
--- a/sd_checklist_meta2.xlsx
+++ b/sd_checklist_meta2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao_\Documents\João Filipe\Universidade\4º Ano\2º Semestre\SD\Projeto-SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0498587A-0301-46B4-8C62-01BCC130E531}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9206DE-AFCB-4A75-A811-BA9A6559B11B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -285,7 +285,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -304,9 +304,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -719,7 +716,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -763,7 +760,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -788,7 +785,7 @@
   <dimension ref="A1:BR47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" zoomScalePageLayoutView="121" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="13.8"/>
@@ -1387,7 +1384,7 @@
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="3">
@@ -1398,7 +1395,7 @@
       <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="3">
@@ -1409,7 +1406,7 @@
       <c r="A9" s="3">
         <v>5</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="3">
@@ -1420,7 +1417,7 @@
       <c r="A10" s="3">
         <v>5</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="3">
@@ -1431,7 +1428,7 @@
       <c r="A11" s="3">
         <v>5</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="3">
@@ -1442,7 +1439,7 @@
       <c r="A12" s="3">
         <v>5</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="3">
@@ -1453,7 +1450,7 @@
       <c r="A13" s="3">
         <v>5</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="3">
@@ -1464,7 +1461,7 @@
       <c r="A14" s="3">
         <v>7</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="3">
@@ -1475,7 +1472,7 @@
       <c r="A15" s="3">
         <v>5</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="3">
@@ -1486,7 +1483,7 @@
       <c r="A16" s="3">
         <v>5</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="3">
@@ -1497,7 +1494,7 @@
       <c r="A17" s="3">
         <v>5</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="3">

</xml_diff>

<commit_message>
relatório falta meter um paragrafozito sobre os votos na parte das struts
</commit_message>
<xml_diff>
--- a/sd_checklist_meta2.xlsx
+++ b/sd_checklist_meta2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao_\Documents\João Filipe\Universidade\4º Ano\2º Semestre\SD\Projeto-SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEF52BD-7CB8-4474-8009-2B044D6319B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A406DA-15EF-4A08-BA00-D90ED19D9B5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BR47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" zoomScalePageLayoutView="121" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="121" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="13.8"/>
@@ -1822,7 +1822,7 @@
       <c r="A22" s="3">
         <v>5</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="3">
@@ -1844,7 +1844,7 @@
       <c r="A24" s="3">
         <v>5</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="3">
@@ -2136,7 +2136,7 @@
       <c r="A26" s="3">
         <v>5</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="3">
@@ -2147,7 +2147,7 @@
       <c r="A27" s="3">
         <v>5</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="3">

</xml_diff>

<commit_message>
relatório e partilha no fb update
</commit_message>
<xml_diff>
--- a/sd_checklist_meta2.xlsx
+++ b/sd_checklist_meta2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao_\Documents\João Filipe\Universidade\4º Ano\2º Semestre\SD\Projeto-SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A406DA-15EF-4A08-BA00-D90ED19D9B5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752221E8-E0D3-470C-A6D1-D094EED217DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -719,7 +719,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -763,7 +763,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -788,7 +788,7 @@
   <dimension ref="A1:BR47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="121" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="13.8"/>
@@ -2158,7 +2158,7 @@
       <c r="A28" s="3">
         <v>5</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C28" s="3">

</xml_diff>